<commit_message>
Verbindung von GDE mit unserem Projekt Hazard
im Ordner GDE_3_Hazard. Ab nun koennen wir weiter in diesem Ordner
programmieren.
</commit_message>
<xml_diff>
--- a/KVs.xlsx
+++ b/KVs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="14115" windowHeight="6975"/>
@@ -11,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -78,14 +78,14 @@
     <t>01xx</t>
   </si>
   <si>
-    <t>0x0x</t>
+    <t>[</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,7 +544,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1790700" y="0"/>
+          <a:off x="3524250" y="0"/>
           <a:ext cx="161925" cy="342899"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -846,7 +846,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -920,7 +920,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -955,7 +954,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1131,19 +1129,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="3.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1181,7 +1179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1228,7 +1226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1275,7 +1273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1322,7 +1320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1369,7 +1367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1377,7 +1375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="H9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1385,7 +1383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="H10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1393,7 +1391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="H11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1401,7 +1399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1407,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="O13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1425,24 +1423,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>